<commit_message>
logboek + instructies voor vraaggenerator
</commit_message>
<xml_diff>
--- a/Drive/Logboeken/Logboek Mark Jan van Lieburg.xlsx
+++ b/Drive/Logboeken/Logboek Mark Jan van Lieburg.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="11955"/>
+    <workbookView xWindow="630" yWindow="600" windowWidth="18570" windowHeight="11370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>Datum</t>
   </si>
@@ -86,6 +86,30 @@
   </si>
   <si>
     <t>Opruimen van projectbestand op GitHub</t>
+  </si>
+  <si>
+    <t>Teambespreking</t>
+  </si>
+  <si>
+    <t>Teambespreking en programmeren</t>
+  </si>
+  <si>
+    <t>Programmeren + tutorials bekijken</t>
+  </si>
+  <si>
+    <t>Groepsgesprek, programmeren + tutorials</t>
+  </si>
+  <si>
+    <t>Programmeren + nadenken</t>
+  </si>
+  <si>
+    <t>Begeleidergesprek + programmeren</t>
+  </si>
+  <si>
+    <t>Programmeren + groepsgesprek</t>
+  </si>
+  <si>
+    <t>Vraaggenereren voorbereiden en instructie schrijven</t>
   </si>
 </sst>
 </file>
@@ -433,7 +457,7 @@
   <dimension ref="A1:W1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -467,8 +491,8 @@
         <v>22</v>
       </c>
       <c r="W2">
-        <f xml:space="preserve"> SUM(D2:D100)</f>
-        <v>39.5</v>
+        <f xml:space="preserve"> SUM(D:D)</f>
+        <v>106.5</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -716,78 +740,230 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="1"/>
+      <c r="A24" s="2">
+        <v>42358</v>
+      </c>
+      <c r="D24" s="4">
+        <v>4</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="1"/>
+      <c r="A25" s="2">
+        <v>42359</v>
+      </c>
+      <c r="D25" s="4">
+        <v>4</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="1"/>
+      <c r="A26" s="2">
+        <v>42360</v>
+      </c>
+      <c r="D26" s="4">
+        <v>6</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="1"/>
+      <c r="A27" s="2">
+        <v>42361</v>
+      </c>
+      <c r="D27" s="4">
+        <v>3</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="1"/>
+      <c r="A28" s="2">
+        <v>42362</v>
+      </c>
+      <c r="D28" s="4">
+        <v>3</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="1"/>
+      <c r="A29" s="2">
+        <v>42363</v>
+      </c>
+      <c r="D29" s="4">
+        <v>3</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="1"/>
+      <c r="A30" s="2">
+        <v>42365</v>
+      </c>
+      <c r="D30" s="4">
+        <v>4</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="1"/>
+      <c r="A31" s="2">
+        <v>42366</v>
+      </c>
+      <c r="D31">
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="1"/>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="1"/>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="A32" s="2">
+        <v>42366</v>
+      </c>
+      <c r="D32" s="4">
+        <v>3</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="2">
+        <v>42367</v>
+      </c>
+      <c r="D33" s="4">
+        <v>5</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="2">
+        <v>42368</v>
+      </c>
+      <c r="D34" s="4">
+        <v>6</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="2">
+        <v>42369</v>
+      </c>
+      <c r="D35" s="4">
+        <v>1</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="2">
+        <v>42372</v>
+      </c>
+      <c r="D36" s="4">
+        <v>4</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="2">
+        <v>42373</v>
+      </c>
+      <c r="D37" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="2">
+        <v>42374</v>
+      </c>
+      <c r="D38" s="4">
+        <v>6</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="2">
+        <v>42375</v>
+      </c>
+      <c r="D39" s="4">
+        <v>2</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="2">
+        <v>42375</v>
+      </c>
+      <c r="D40" s="4">
+        <v>2</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="2">
+        <v>42376</v>
+      </c>
+      <c r="D41" s="4">
+        <v>3</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="2">
+        <v>42376</v>
+      </c>
+      <c r="D42" s="4">
+        <v>1</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:7">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:7">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:7">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:7">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:7">
       <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:1">

</xml_diff>